<commit_message>
changes after Jan 23 lecture
</commit_message>
<xml_diff>
--- a/schedule/schedule.xlsx
+++ b/schedule/schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t xml:space="preserve">Tuesday</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">P2</t>
   </si>
   <si>
+    <t xml:space="preserve">W3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longitudinal Trim and Stability (2.4)</t>
   </si>
   <si>
@@ -85,9 +88,6 @@
     <t xml:space="preserve">Longitudinal Linear Model (4.9-4.10)</t>
   </si>
   <si>
-    <t xml:space="preserve">W3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Longitudinal Modes (6.2)</t>
   </si>
   <si>
@@ -97,13 +97,16 @@
     <t xml:space="preserve">P3</t>
   </si>
   <si>
+    <t xml:space="preserve">W4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Longitudinal Control (7.1-7.7)</t>
   </si>
   <si>
     <t xml:space="preserve">Lateral Forces and Moments</t>
   </si>
   <si>
-    <t xml:space="preserve">W4</t>
+    <t xml:space="preserve">W5</t>
   </si>
   <si>
     <t xml:space="preserve">Exam 2</t>
@@ -127,7 +130,7 @@
     <t xml:space="preserve">Lateral Stability Augmentation (7.8-7.12)</t>
   </si>
   <si>
-    <t xml:space="preserve">W5</t>
+    <t xml:space="preserve">W6</t>
   </si>
   <si>
     <t xml:space="preserve">Lateral Guidance and Control (8.1-8.9)</t>
@@ -136,7 +139,7 @@
     <t xml:space="preserve">Introduction to Optimal Control (LQR)</t>
   </si>
   <si>
-    <t xml:space="preserve">W6</t>
+    <t xml:space="preserve">W7</t>
   </si>
   <si>
     <t xml:space="preserve">Human Factors (1.3-1.5)</t>
@@ -434,20 +437,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="2.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.54"/>
   </cols>
@@ -584,6 +587,12 @@
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -594,7 +603,7 @@
         <v>45342</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="n">
@@ -602,7 +611,7 @@
         <v>45344</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -616,7 +625,7 @@
         <v>45349</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="n">
@@ -624,11 +633,17 @@
         <v>45351</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -654,6 +669,12 @@
       <c r="H9" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -664,7 +685,7 @@
         <v>45363</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="n">
@@ -672,11 +693,17 @@
         <v>45365</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -688,7 +715,7 @@
         <v>45370</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="n">
@@ -696,7 +723,7 @@
         <v>45372</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -726,7 +753,7 @@
         <v>45384</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="n">
@@ -734,11 +761,17 @@
         <v>45386</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -750,7 +783,7 @@
         <v>45391</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="n">
@@ -758,11 +791,17 @@
         <v>45393</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -774,7 +813,7 @@
         <v>45398</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="n">
@@ -782,11 +821,14 @@
         <v>45400</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -798,7 +840,7 @@
         <v>45405</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="n">
@@ -806,11 +848,14 @@
         <v>45407</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -822,7 +867,7 @@
         <v>45412</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4" t="n">
@@ -830,7 +875,7 @@
         <v>45414</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -841,7 +886,7 @@
         <v>45416</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>

</xml_diff>

<commit_message>
updated schedule for two Ws
</commit_message>
<xml_diff>
--- a/schedule/schedule.xlsx
+++ b/schedule/schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">Tuesday</t>
   </si>
@@ -70,85 +70,82 @@
     <t xml:space="preserve">Longitudinal Forces and Moments (2.1-2.3)</t>
   </si>
   <si>
+    <t xml:space="preserve">W3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal Trim and Stability (2.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal Stability Derivatives (5.1-5.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal Linear Model (4.9-4.10)</t>
+  </si>
+  <si>
     <t xml:space="preserve">P2</t>
   </si>
   <si>
-    <t xml:space="preserve">W3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitudinal Trim and Stability (2.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exam 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitudinal Stability Derivatives (5.1-5.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitudinal Linear Model (4.9-4.10)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Longitudinal Modes (6.2)</t>
   </si>
   <si>
     <t xml:space="preserve">Mode Approximations (6.3)</t>
   </si>
   <si>
+    <t xml:space="preserve">W4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitudinal Control (7.1-7.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral Forces and Moments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dihedral Effect (5.6-5.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordinated Turn (3.8-3.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral Modes (6.7)</t>
+  </si>
+  <si>
     <t xml:space="preserve">P3</t>
   </si>
   <si>
-    <t xml:space="preserve">W4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Longitudinal Control (7.1-7.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral Forces and Moments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exam 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dihedral Effect (5.6-5.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordinated Turn (3.8-3.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral Modes (6.7)</t>
+    <t xml:space="preserve">Lateral Modal Approximations (6.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral Stability Augmentation (7.8-7.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lateral Guidance and Control (8.1-8.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Optimal Control (LQR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Factors (1.3-1.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmosphere and Wind (6.9)</t>
   </si>
   <si>
     <t xml:space="preserve">P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral Modal Approximations (6.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral Stability Augmentation (7.8-7.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lateral Guidance and Control (8.1-8.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Optimal Control (LQR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Factors (1.3-1.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atmosphere and Wind (6.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P5</t>
   </si>
   <si>
     <t xml:space="preserve">Review</t>
@@ -275,7 +272,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,6 +318,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,10 +438,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,12 +588,6 @@
       <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -603,7 +598,7 @@
         <v>45342</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4" t="n">
@@ -611,7 +606,7 @@
         <v>45344</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -625,7 +620,7 @@
         <v>45349</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4" t="n">
@@ -633,18 +628,13 @@
         <v>45351</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -666,15 +656,10 @@
         <v>23</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -685,26 +670,21 @@
         <v>45363</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4" t="n">
         <f aca="false">B10+2</f>
         <v>45365</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -714,35 +694,35 @@
         <f aca="false">B10+7</f>
         <v>45370</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>29</v>
+      <c r="C11" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="4" t="n">
         <f aca="false">B11+2</f>
         <v>45372</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>30</v>
+      <c r="F11" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16" t="n">
+      <c r="A12" s="16"/>
+      <c r="B12" s="17" t="n">
         <f aca="false">B11+7</f>
         <v>45377</v>
       </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16" t="n">
+      <c r="D12" s="16"/>
+      <c r="E12" s="17" t="n">
         <f aca="false">B12+2</f>
         <v>45379</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -752,27 +732,22 @@
         <f aca="false">B12+7</f>
         <v>45384</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>31</v>
+      <c r="C13" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="4" t="n">
         <f aca="false">B13+2</f>
         <v>45386</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -782,27 +757,22 @@
         <f aca="false">B13+7</f>
         <v>45391</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>34</v>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4" t="n">
         <f aca="false">B14+2</f>
         <v>45393</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -812,24 +782,22 @@
         <f aca="false">B14+7</f>
         <v>45398</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>37</v>
+      <c r="C15" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4" t="n">
         <f aca="false">B15+2</f>
         <v>45400</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -839,24 +807,22 @@
         <f aca="false">B15+7</f>
         <v>45405</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>40</v>
+      <c r="C16" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4" t="n">
         <f aca="false">B16+2</f>
         <v>45407</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -866,8 +832,8 @@
         <f aca="false">B16+7</f>
         <v>45412</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>43</v>
+      <c r="C17" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="4" t="n">
@@ -875,7 +841,7 @@
         <v>45414</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -885,8 +851,8 @@
       <c r="B18" s="4" t="n">
         <v>45416</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>44</v>
+      <c r="C18" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -895,16 +861,16 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="20"/>
+      <c r="B19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="20"/>
+      <c r="B20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="20"/>
+      <c r="B21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="20"/>
+      <c r="B22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>